<commit_message>
Update results with new concentrations
</commit_message>
<xml_diff>
--- a/Datos/concentraciones_contaminantes.xlsx
+++ b/Datos/concentraciones_contaminantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Uni\ArchivosProgra\OPTI\Entrega2Opti\Listos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maitevillagran/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39E42E5-5EE2-456B-985A-3F5494FBA8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{953305BC-2E4C-8A46-B74F-96F1E6294996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="6825" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7120" yWindow="5240" windowWidth="21600" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,18 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -72,7 +76,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,37 +414,38 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>5.7054</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>833</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2.7397</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1.8355999999999999</v>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0.10349999999999999</v>
+        <v>7.0300000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1.5525</v>
+        <f>67</f>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>